<commit_message>
setting a node.js environment
</commit_message>
<xml_diff>
--- a/DataBox/DataTable.xlsx
+++ b/DataBox/DataTable.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>minchul</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>minchulTEST</t>
+  </si>
+  <si>
+    <t>sdgsdgsd</t>
+  </si>
+  <si>
+    <t>minchulTESTsetset</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="H12" sqref="H12"/>
@@ -426,6 +432,22 @@
       </c>
       <c r="B11">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1234567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>